<commit_message>
before doing g final thing
</commit_message>
<xml_diff>
--- a/public_html/time/ArnavBansal_timesheet.xlsx
+++ b/public_html/time/ArnavBansal_timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PRJ566\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67A6D04-B9AF-4A5F-9C4A-67B6DECCEA3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44551E5-4554-413F-8780-DCDFFCCABBDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18210" tabRatio="748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="59">
   <si>
     <t>Status</t>
   </si>
@@ -215,19 +215,31 @@
     <t>Domain class Diagram</t>
   </si>
   <si>
-    <r>
-      <t>PRJ666 - Timesheet - Group</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
+    <t>Posted On:     March 18, 2019</t>
+  </si>
+  <si>
+    <t>Domain class diagram update</t>
+  </si>
+  <si>
+    <t>Use cases updated</t>
+  </si>
+  <si>
+    <t>Posted On:     March 4, 2019</t>
+  </si>
+  <si>
+    <t>document formatting</t>
+  </si>
+  <si>
+    <t>Posted On:     March 25, 2019</t>
+  </si>
+  <si>
+    <t>Database optimization research</t>
+  </si>
+  <si>
+    <t>Database create table scripts</t>
+  </si>
+  <si>
+    <t>Document review and proofreading for 7.0+</t>
   </si>
 </sst>
 </file>
@@ -2615,7 +2627,7 @@
   <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6117,7 +6129,7 @@
       </c>
       <c r="F14" s="41">
         <f>'Jan-21'!F33+'Jan-28'!F33+'Feb-04'!F33+'Feb-11'!F33+'Feb-17'!F33+'Feb-25'!F33+'Mar-11'!F33+'Mar-18'!F33+'Mar-25'!F33+'Apr-01'!F33+'Apr-08'!F33</f>
-        <v>6.416666666666667</v>
+        <v>11.666666666666668</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -9378,7 +9390,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C9"/>
+      <selection activeCell="C5" sqref="C5:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11334,7 +11346,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11448,7 +11460,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="23"/>
       <c r="C5" s="51" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -11495,7 +11507,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="23"/>
       <c r="C7" s="51" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="17"/>
@@ -11543,7 +11555,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="23"/>
       <c r="C9" s="51" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="17"/>
@@ -11656,10 +11668,18 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="55">
+        <v>43527</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -11968,7 +11988,7 @@
       </c>
       <c r="F33" s="41">
         <f>SUM(F14:F31)/60</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -12291,7 +12311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBD318F-CC41-49E7-B3A6-51489FF13BC4}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12403,8 +12425,8 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="16" t="s">
-        <v>14</v>
+      <c r="C5" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -12450,8 +12472,8 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="16" t="s">
-        <v>17</v>
+      <c r="C7" s="51" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="17"/>
@@ -12498,8 +12520,8 @@
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="16" t="s">
-        <v>7</v>
+      <c r="C9" s="51" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="17"/>
@@ -12612,11 +12634,17 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
+      <c r="C14" s="53">
+        <v>43540</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="3">
+        <v>30</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -12630,10 +12658,18 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="53">
+        <v>43541</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -12926,7 +12962,7 @@
       </c>
       <c r="F33" s="41">
         <f>SUM(F14:F31)/60</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -13249,7 +13285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41223AE2-D6CA-449D-84C8-AA9FDE8BBAF2}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13361,8 +13399,8 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="16" t="s">
-        <v>14</v>
+      <c r="C5" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -13408,8 +13446,8 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="16" t="s">
-        <v>17</v>
+      <c r="C7" s="51" t="s">
+        <v>55</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="17"/>
@@ -13456,8 +13494,8 @@
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="16" t="s">
-        <v>7</v>
+      <c r="C9" s="51" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="17"/>
@@ -13570,11 +13608,17 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
+      <c r="C14" s="53">
+        <v>43546</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="3">
+        <v>120</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -13588,10 +13632,18 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="53">
+        <v>43547</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -13604,10 +13656,18 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="53">
+        <v>43548</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3">
+        <v>30</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -13884,7 +13944,7 @@
       </c>
       <c r="F33" s="41">
         <f>SUM(F14:F31)/60</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>

</xml_diff>